<commit_message>
Project Completed, Final Changes
</commit_message>
<xml_diff>
--- a/MOMTracker/MOMTracker/STUDENTS.xlsx
+++ b/MOMTracker/MOMTracker/STUDENTS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B997675A-8A59-4945-B978-0D4F1E409F12}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74558456-82B5-48BB-BA14-9A5B046976A6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4800" yWindow="2870" windowWidth="14400" windowHeight="7450" xr2:uid="{61A34FAA-58C0-4689-83DA-A4B271E25900}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10540" xr2:uid="{61A34FAA-58C0-4689-83DA-A4B271E25900}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,61 +31,78 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
-  <si>
-    <t>STATUS</t>
-  </si>
-  <si>
-    <t>STATUSREM</t>
-  </si>
-  <si>
-    <t>EXPECTEDCLOSURE</t>
-  </si>
-  <si>
-    <t>RESP</t>
-  </si>
-  <si>
-    <t>ACTIONABLE</t>
-  </si>
-  <si>
-    <t>REVIEWDATE</t>
-  </si>
-  <si>
-    <t>ITEM</t>
-  </si>
-  <si>
-    <t>CSBI</t>
-  </si>
-  <si>
-    <t>CD</t>
-  </si>
-  <si>
-    <t>VZDBS</t>
-  </si>
-  <si>
-    <t>VDBVSH</t>
-  </si>
-  <si>
-    <t>j</t>
-  </si>
-  <si>
-    <t>h</t>
-  </si>
-  <si>
-    <t>DUIHCnew</t>
-  </si>
-  <si>
-    <t>jnew</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
+  <si>
+    <t>CURRENTSTAGE</t>
+  </si>
+  <si>
+    <t>RESPONSIBILITY</t>
+  </si>
+  <si>
+    <t>TARGET</t>
+  </si>
+  <si>
+    <t>ITSPOC</t>
+  </si>
+  <si>
+    <t>TASKDESCRIPTION</t>
+  </si>
+  <si>
+    <t>ACTIONPOINT</t>
+  </si>
+  <si>
+    <t>EMAIL</t>
+  </si>
+  <si>
+    <t>NEW SOMETHING</t>
+  </si>
+  <si>
+    <t>EXAMPLE 1</t>
+  </si>
+  <si>
+    <t>RAM</t>
+  </si>
+  <si>
+    <t>swasti.tiwari@gmail.com</t>
+  </si>
+  <si>
+    <t>NEW SOMETHING 2</t>
+  </si>
+  <si>
+    <t>example 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">exampl2 </t>
+  </si>
+  <si>
+    <t>abc</t>
+  </si>
+  <si>
+    <t>3as1827000176@gmail.com</t>
+  </si>
+  <si>
+    <t>USER1</t>
+  </si>
+  <si>
+    <t>USER2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -108,14 +125,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -431,37 +451,37 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="11.81640625" customWidth="1"/>
+    <col min="1" max="2" width="16.81640625" customWidth="1"/>
     <col min="3" max="3" width="17.81640625" customWidth="1"/>
     <col min="4" max="4" width="16.7265625" customWidth="1"/>
     <col min="5" max="5" width="13.54296875" customWidth="1"/>
     <col min="6" max="6" width="11.90625" customWidth="1"/>
-    <col min="7" max="7" width="15.6328125" customWidth="1"/>
+    <col min="7" max="7" width="24.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F1" t="s">
         <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
       </c>
       <c r="G1" t="s">
         <v>6</v>
@@ -469,13 +489,13 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="1">
-        <v>41255</v>
+      <c r="C2" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>8</v>
@@ -484,33 +504,33 @@
         <v>9</v>
       </c>
       <c r="F2" s="1">
-        <v>40461</v>
-      </c>
-      <c r="G2" s="1" t="s">
+        <v>44177</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B3" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="1">
-        <v>40097</v>
+      <c r="C3" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F3" s="1">
-        <v>39332</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>11</v>
+        <v>44177</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
@@ -518,6 +538,10 @@
       <c r="F4" s="1"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G2" r:id="rId1" xr:uid="{2594D7B3-AA3D-4DBE-BE02-5088A36E37F7}"/>
+    <hyperlink ref="G3" r:id="rId2" xr:uid="{BBA1D0A7-4F5C-4F9A-9EFC-D802373C5F34}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>